<commit_message>
Poprawione zdania z rekcja Dentysta - slownictwo Bank - slownictwo (poprawione)
</commit_message>
<xml_diff>
--- a/rektion/rektion-sätze.xlsx
+++ b/rektion/rektion-sätze.xlsx
@@ -177,9 +177,6 @@
     <t>Ich setze mich für deinen Vorschlag ein.</t>
   </si>
   <si>
-    <t>Wir haben uns für diesen Termin entscheiden.</t>
-  </si>
-  <si>
     <t>Er entschuldigt sich bei mir für die Verspätung.</t>
   </si>
   <si>
@@ -771,9 +768,6 @@
     <t>Co rozumie się pod tym pojęciem?</t>
   </si>
   <si>
-    <t>Kiedy się o tym dowiedziałeś?</t>
-  </si>
-  <si>
     <t>To zależy ode mnie.</t>
   </si>
   <si>
@@ -792,15 +786,9 @@
     <t>Ich habe nichts von dem Buch gehört.</t>
   </si>
   <si>
-    <t>Nic nie słyszałem o tej książce.</t>
-  </si>
-  <si>
     <t>O czym traktuje ten tekst?</t>
   </si>
   <si>
-    <t>Dużo skorzystałem na tej praktyce.</t>
-  </si>
-  <si>
     <t>O czym rozmawiacie?</t>
   </si>
   <si>
@@ -825,9 +813,6 @@
     <t>Der Besuch hat zu der Vertiefung der Beziehungen beigetragen.</t>
   </si>
   <si>
-    <t>Odwiedziny przyczyniły się do pogłębienia relacji.</t>
-  </si>
-  <si>
     <t>Matura uprawnia do studiów.</t>
   </si>
   <si>
@@ -837,12 +822,6 @@
     <t>Nie potrafię się na to zdecydować.</t>
   </si>
   <si>
-    <t>Ten kraj rozwinął się w kraj przemysłowy.</t>
-  </si>
-  <si>
-    <t>Do czego doprowadziła ta polityka?</t>
-  </si>
-  <si>
     <t>To należy do twoich zadań.</t>
   </si>
   <si>
@@ -945,15 +924,9 @@
     <t>Dziś spotykamy się z dobrymi przyjaciółmi.</t>
   </si>
   <si>
-    <t>Peter rozstał się ze swoim przyjacielem.</t>
-  </si>
-  <si>
     <t>Czy może mnie pan połączyć z sekretariatem?</t>
   </si>
   <si>
-    <t>Dziś Jens zaręczył się ze swoją dziewczyną.</t>
-  </si>
-  <si>
     <t>On pracuje nad swoim projektem.</t>
   </si>
   <si>
@@ -1032,9 +1005,6 @@
     <t>Pytam go o jego adres.</t>
   </si>
   <si>
-    <t>Bardzo się zdenerwowaliśmy tym incydentem.</t>
-  </si>
-  <si>
     <t>On panował długo nad tym krajem. (prät.)</t>
   </si>
   <si>
@@ -1083,18 +1053,12 @@
     <t>On pomaga jej w ucieczce.</t>
   </si>
   <si>
-    <t>Niektórzy ludzie czują wstręt do pająka.</t>
-  </si>
-  <si>
     <t>Mąkę i proszek do pieczenia miesza się z jajkami i cukrem.</t>
   </si>
   <si>
     <t>Niektóre związki rozsypują się z powodu rutyny.</t>
   </si>
   <si>
-    <t>Die Qualität des neues Artikels weicht von der des altes ab.</t>
-  </si>
-  <si>
     <t>Jakość nowego artykułu odbiega od starego.</t>
   </si>
   <si>
@@ -1134,9 +1098,6 @@
     <t>Teraz trzeba się uzbroić w cierpliwość.</t>
   </si>
   <si>
-    <t>Die Anzahl den Teilnehmern wurde auf zwanzig begrenzt.</t>
-  </si>
-  <si>
     <t>Ich beschränke mich auf das Notwendigste.</t>
   </si>
   <si>
@@ -1221,9 +1182,6 @@
     <t>On narzeka na zbyt małe zarobki. (bek.)</t>
   </si>
   <si>
-    <t>Er solte sich darüber nicht wundern.</t>
-  </si>
-  <si>
     <t>Nie powinno go to dziwić.</t>
   </si>
   <si>
@@ -1257,9 +1215,6 @@
     <t>Co o tym myślisz? (d.)</t>
   </si>
   <si>
-    <t>Ich bin neugierich daran, was er sagen wird.</t>
-  </si>
-  <si>
     <t>Jestem ciekawy, co on na to powie.</t>
   </si>
   <si>
@@ -1320,9 +1275,6 @@
     <t>Ich znajomość sięga wspólnych zajęć na uniwersytecie.</t>
   </si>
   <si>
-    <t>Sie stauen über die Architektur der Stadt.</t>
-  </si>
-  <si>
     <t>Oni są zadziwieni architekturą miasta.</t>
   </si>
   <si>
@@ -1335,9 +1287,6 @@
     <t>Man hat ihn aus der Partei ausgeschlossen.</t>
   </si>
   <si>
-    <t>On został wykluczony z partii.</t>
-  </si>
-  <si>
     <t>Wir protestieren gegen die Kinderarbeit.</t>
   </si>
   <si>
@@ -1392,15 +1341,9 @@
     <t>On choruje na grypę.</t>
   </si>
   <si>
-    <t>Sie wird nicht dazu äußern.</t>
-  </si>
-  <si>
     <t>Ona nie wyrazi swojego zdania co do tego.</t>
   </si>
   <si>
-    <t>Sie hat sich sehr für dir Rechte von Kindern engagiert.</t>
-  </si>
-  <si>
     <t>Ona zaangażowała się bardzo w kwestię praw dziecka. (perf.)</t>
   </si>
   <si>
@@ -1431,9 +1374,6 @@
     <t>Samochód zderzył się z tramwajem. (perf.)</t>
   </si>
   <si>
-    <t>Ona przestraszyła się własnego cienia.</t>
-  </si>
-  <si>
     <t>Sie hat sich vor dem eigenen Schatten erschreckt.</t>
   </si>
   <si>
@@ -1494,9 +1434,6 @@
     <t>Sie hat sich hinter einer Zeitung verschänzt.</t>
   </si>
   <si>
-    <t>Ukryła się (swoją twarz) za gazetą.</t>
-  </si>
-  <si>
     <t>Sie ist begeistert von ihrem Schwiegersohn.</t>
   </si>
   <si>
@@ -1515,9 +1452,6 @@
     <t>Jeder stöhnt unter der Hitze.</t>
   </si>
   <si>
-    <t>Każdy narzeka z powodu upałów.</t>
-  </si>
-  <si>
     <t>Meine Eltern sind wütend auf mich.</t>
   </si>
   <si>
@@ -1654,6 +1588,72 @@
   </si>
   <si>
     <t>Sie ist über ihre Ratlosigkeit verärgert.</t>
+  </si>
+  <si>
+    <t>Er sollte sich darüber nicht wundern.</t>
+  </si>
+  <si>
+    <t>Wir haben uns für diesen Termin entschieden.</t>
+  </si>
+  <si>
+    <t>Niektórzy ludzie brzydzą się pająka.</t>
+  </si>
+  <si>
+    <t>Dziś Jens zaręczył się ze swoją dziewczyną. (perf.)</t>
+  </si>
+  <si>
+    <t>Ich bin neugierig daran, was er sagen wird.</t>
+  </si>
+  <si>
+    <t>Sie staunen über die Architektur der Stadt.</t>
+  </si>
+  <si>
+    <t>Die Anzahl der Teilnehmer wurde auf zwanzig begrenzt.</t>
+  </si>
+  <si>
+    <t>Sie wird sich nicht dazu äußern.</t>
+  </si>
+  <si>
+    <t>Każdy narzeka z powodu upału.</t>
+  </si>
+  <si>
+    <t>Sie hat sich sehr für die Rechte von Kindern engagiert.</t>
+  </si>
+  <si>
+    <t>Die Qualität des neuen Artikels weicht von der des alten ab.</t>
+  </si>
+  <si>
+    <t>Bardzo się zdenerwowaliśmy tym incydentem. (perf.)</t>
+  </si>
+  <si>
+    <t>Kiedy się o tym dowiedziałeś? (perf.)</t>
+  </si>
+  <si>
+    <t>Nic nie słyszałem o tej książce. (perf.)</t>
+  </si>
+  <si>
+    <t>Dużo skorzystałem na tej praktyce. (perf.)</t>
+  </si>
+  <si>
+    <t>Odwiedziny przyczyniły się do pogłębienia relacji. (perf.)</t>
+  </si>
+  <si>
+    <t>Ten kraj rozwinął się w kraj przemysłowy. (perf.)</t>
+  </si>
+  <si>
+    <t>Do czego doprowadziła ta polityka? (perf.)</t>
+  </si>
+  <si>
+    <t>Peter rozstał się ze swoim przyjacielem. (perf.)</t>
+  </si>
+  <si>
+    <t>On został wykluczony z partii. (perf.)</t>
+  </si>
+  <si>
+    <t>Ona przestraszyła się własnego cienia. (perf.)</t>
+  </si>
+  <si>
+    <t>Ukryła się (swoją twarz) za gazetą. (perf.)</t>
   </si>
 </sst>
 </file>
@@ -2003,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2019,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="27.6" customHeight="1">
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27.6" customHeight="1">
@@ -2035,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" customHeight="1">
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" customHeight="1">
@@ -2051,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" customHeight="1">
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="27.6" customHeight="1">
@@ -2067,7 +2067,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" customHeight="1">
@@ -2075,15 +2075,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" customHeight="1">
@@ -2091,7 +2091,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" customHeight="1">
@@ -2099,7 +2099,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="27.6" customHeight="1">
@@ -2107,7 +2107,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="27.6" customHeight="1">
@@ -2115,15 +2115,15 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="27.6" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="27.6" customHeight="1">
@@ -2131,7 +2131,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27.6" customHeight="1">
@@ -2139,7 +2139,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="27.6" customHeight="1">
@@ -2147,15 +2147,15 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="27.6" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="27.6" customHeight="1">
@@ -2163,23 +2163,23 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="27.6" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="27.6" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="27.6" customHeight="1">
@@ -2187,7 +2187,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="27.6" customHeight="1">
@@ -2195,7 +2195,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="27.6" customHeight="1">
@@ -2203,15 +2203,15 @@
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="27.6" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="27.6" customHeight="1">
@@ -2219,15 +2219,15 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="27.6" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="27.6" customHeight="1">
@@ -2235,7 +2235,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="27.6" customHeight="1">
@@ -2243,15 +2243,15 @@
         <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="27.6" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="27.6" customHeight="1">
@@ -2259,7 +2259,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="27.6" customHeight="1">
@@ -2267,7 +2267,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="27.6" customHeight="1">
@@ -2275,7 +2275,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="27.6" customHeight="1">
@@ -2283,7 +2283,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="27.6" customHeight="1">
@@ -2291,31 +2291,31 @@
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="27.6" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="27.6" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="27.6" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>372</v>
+      <c r="A38" s="6" t="s">
+        <v>530</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="27.6" customHeight="1">
@@ -2323,23 +2323,23 @@
         <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="27.6" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="27.6" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="27.6" customHeight="1">
@@ -2347,7 +2347,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="27.6" customHeight="1">
@@ -2355,7 +2355,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="27.6" customHeight="1">
@@ -2363,7 +2363,7 @@
         <v>30</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="27.6" customHeight="1">
@@ -2371,7 +2371,7 @@
         <v>31</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="27.6" customHeight="1">
@@ -2379,15 +2379,15 @@
         <v>32</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="27.6" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="27.6" customHeight="1">
@@ -2395,15 +2395,15 @@
         <v>33</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="27.6" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="27.6" customHeight="1">
@@ -2411,7 +2411,7 @@
         <v>34</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="27.6" customHeight="1">
@@ -2419,7 +2419,7 @@
         <v>35</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="27.6" customHeight="1">
@@ -2427,15 +2427,15 @@
         <v>36</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="27.6" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="27.6" customHeight="1">
@@ -2443,7 +2443,7 @@
         <v>37</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="27.6" customHeight="1">
@@ -2451,7 +2451,7 @@
         <v>38</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="27.6" customHeight="1">
@@ -2459,23 +2459,23 @@
         <v>39</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="27.6" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="27.6" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="27.6" customHeight="1">
@@ -2483,7 +2483,7 @@
         <v>40</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="27.6" customHeight="1">
@@ -2491,15 +2491,15 @@
         <v>41</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="27.6" customHeight="1">
       <c r="A61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="27.6" customHeight="1">
@@ -2507,7 +2507,7 @@
         <v>42</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="27.6" customHeight="1">
@@ -2515,7 +2515,7 @@
         <v>43</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="27.6" customHeight="1">
@@ -2523,15 +2523,15 @@
         <v>44</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="27.6" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="27.6" customHeight="1">
@@ -2539,7 +2539,7 @@
         <v>45</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="27.6" customHeight="1">
@@ -2547,7 +2547,7 @@
         <v>46</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="27.6" customHeight="1">
@@ -2555,7 +2555,7 @@
         <v>47</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="27.6" customHeight="1">
@@ -2563,7 +2563,7 @@
         <v>48</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="27.6" customHeight="1">
@@ -2571,15 +2571,15 @@
         <v>49</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="27.6" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="27.6" customHeight="1">
@@ -2587,7 +2587,7 @@
         <v>50</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="27.6" customHeight="1">
@@ -2595,7 +2595,7 @@
         <v>51</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="27.6" customHeight="1">
@@ -2603,1601 +2603,1601 @@
         <v>52</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="27.6" customHeight="1">
-      <c r="A75" s="1" t="s">
-        <v>53</v>
+      <c r="A75" s="6" t="s">
+        <v>525</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="27.6" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="27.6" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="27.6" customHeight="1">
       <c r="A78" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="27.6" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="27.6" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="27.6" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="27.6" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="27.6" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="27.6" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="27.6" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="27.6" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="27.6" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="27.6" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="27.6" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="27.6" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="27.6" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="27.6" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="27.6" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="27.6" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="27.6" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="27.6" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="27.6" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="27.6" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="27.6" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="27.6" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="27.6" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>468</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="27.6" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="27.6" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="27.6" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="27.6" customHeight="1">
       <c r="A105" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="27.6" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>469</v>
+        <v>450</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="27.6" customHeight="1">
       <c r="A107" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="27.6" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>470</v>
+        <v>451</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="27.6" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="27.6" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="27.6" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="27.6" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="27.6" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="27.6" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="27.6" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="27.6" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="27.6" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="27.6" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="27.6" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="27.6" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="27.6" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="27.6" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>338</v>
+        <v>91</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="27.6" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="27.6" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="27.6" customHeight="1">
       <c r="A125" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="27.6" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="27.6" customHeight="1">
       <c r="A127" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="27.6" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="27.6" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="27.6" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="27.6" customHeight="1">
       <c r="A131" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="27.6" customHeight="1">
       <c r="A132" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="27.6" customHeight="1">
       <c r="A133" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="27.6" customHeight="1">
       <c r="A134" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="27.6" customHeight="1">
       <c r="A135" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="27.6" customHeight="1">
       <c r="A136" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="27.6" customHeight="1">
       <c r="A137" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="27.6" customHeight="1">
       <c r="A138" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="27.6" customHeight="1">
-      <c r="A139" s="1" t="s">
-        <v>401</v>
+      <c r="A139" s="6" t="s">
+        <v>524</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="27.6" customHeight="1">
       <c r="A140" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="27.6" customHeight="1">
       <c r="A141" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="27.6" customHeight="1">
       <c r="A142" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="27.6" customHeight="1">
       <c r="A143" s="1" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="27.6" customHeight="1">
       <c r="A144" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="27.6" customHeight="1">
       <c r="A145" s="1" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="27.6" customHeight="1">
       <c r="A146" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="27.6" customHeight="1">
       <c r="A147" s="1" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="27.6" customHeight="1">
       <c r="A148" s="1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="27.6" customHeight="1">
       <c r="A149" s="1" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="27.6" customHeight="1">
       <c r="A150" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="27.6" customHeight="1">
       <c r="A151" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="27.6" customHeight="1">
       <c r="A152" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="27.6" customHeight="1">
       <c r="A153" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="27.6" customHeight="1">
       <c r="A154" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="27.6" customHeight="1">
       <c r="A155" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="27.6" customHeight="1">
       <c r="A156" s="1" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="27.6" customHeight="1">
       <c r="A157" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>251</v>
+        <v>112</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="27.6" customHeight="1">
       <c r="A158" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="27.6" customHeight="1">
       <c r="A159" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="27.6" customHeight="1">
       <c r="A160" s="1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="27.6" customHeight="1">
       <c r="A161" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="27.6" customHeight="1">
       <c r="A162" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="27.6" customHeight="1">
       <c r="A163" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>260</v>
+        <v>337</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="27.6" customHeight="1">
       <c r="A164" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="27.6" customHeight="1">
       <c r="A165" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="27.6" customHeight="1">
       <c r="A166" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="27.6" customHeight="1">
       <c r="A167" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="27.6" customHeight="1">
       <c r="A168" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="27.6" customHeight="1">
       <c r="A169" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="27.6" customHeight="1">
       <c r="A170" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="27.6" customHeight="1">
       <c r="A171" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="27.6" customHeight="1">
       <c r="A172" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="27.6" customHeight="1">
       <c r="A173" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="27.6" customHeight="1">
       <c r="A174" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="27.6" customHeight="1">
       <c r="A175" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="27.6" customHeight="1">
       <c r="A176" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="27.6" customHeight="1">
       <c r="A177" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="27.6" customHeight="1">
       <c r="A178" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="27.6" customHeight="1">
       <c r="A179" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>273</v>
+        <v>128</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="27.6" customHeight="1">
       <c r="A180" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>274</v>
+        <v>129</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="27.6" customHeight="1">
       <c r="A181" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="27.6" customHeight="1">
       <c r="A182" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="27.6" customHeight="1">
       <c r="A183" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="27.6" customHeight="1">
       <c r="A184" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="27.6" customHeight="1">
       <c r="A185" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="27.6" customHeight="1">
       <c r="A186" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="27.6" customHeight="1">
       <c r="A187" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="27.6" customHeight="1">
       <c r="A188" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="27.6" customHeight="1">
       <c r="A189" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="27.6" customHeight="1">
       <c r="A190" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="27.6" customHeight="1">
       <c r="A191" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="27.6" customHeight="1">
       <c r="A192" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="27.6" customHeight="1">
       <c r="A193" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="27.6" customHeight="1">
       <c r="A194" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="27.6" customHeight="1">
       <c r="A195" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>355</v>
+        <v>280</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="27.6" customHeight="1">
       <c r="A196" s="1" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="27.6" customHeight="1">
       <c r="A197" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="27.6" customHeight="1">
       <c r="A198" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="27.6" customHeight="1">
       <c r="A199" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="27.6" customHeight="1">
       <c r="A200" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>309</v>
+        <v>285</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="27.6" customHeight="1">
       <c r="A201" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="27.6" customHeight="1">
       <c r="A202" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>311</v>
+        <v>287</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="27.6" customHeight="1">
       <c r="A203" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="27.6" customHeight="1">
       <c r="A204" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="27.6" customHeight="1">
-      <c r="A205" s="1" t="s">
-        <v>358</v>
+      <c r="A205" s="6" t="s">
+        <v>534</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="27.6" customHeight="1">
-      <c r="A206" s="1" t="s">
-        <v>413</v>
+      <c r="A206" s="6" t="s">
+        <v>528</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="27.6" customHeight="1">
       <c r="A207" s="1" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="208" spans="1:3" s="3" customFormat="1" ht="27.6" customHeight="1">
       <c r="A208" s="2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C208" s="5"/>
     </row>
     <row r="209" spans="1:2" ht="27.6" customHeight="1">
       <c r="A209" s="1" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="27.6" customHeight="1">
       <c r="A210" s="1" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="27.6" customHeight="1">
       <c r="A211" s="1" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="27.6" customHeight="1">
       <c r="A212" s="1" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="27.6" customHeight="1">
       <c r="A213" s="1" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="27.6" customHeight="1">
       <c r="A214" s="1" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="27.6" customHeight="1"/>
     <row r="216" spans="1:2" ht="27.6" customHeight="1">
       <c r="A216" s="1" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="27.6" customHeight="1">
       <c r="A217" s="1" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="27.6" customHeight="1">
       <c r="A218" s="1" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="27.6" customHeight="1">
       <c r="A219" s="1" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="27.6" customHeight="1">
       <c r="A220" s="1" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="27.6" customHeight="1">
       <c r="A221" s="6" t="s">
-        <v>544</v>
+        <v>522</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="27.6" customHeight="1">
       <c r="A222" s="1" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="27.6" customHeight="1">
       <c r="A223" s="1" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="27.6" customHeight="1">
-      <c r="A224" s="1" t="s">
-        <v>434</v>
+      <c r="A224" s="6" t="s">
+        <v>529</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="27.6" customHeight="1">
       <c r="A225" s="1" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="27.6" customHeight="1">
       <c r="A226" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>439</v>
+        <v>422</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="27.6" customHeight="1">
       <c r="A227" s="1" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="27.6" customHeight="1">
       <c r="A228" s="1" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="27.6" customHeight="1">
       <c r="A229" s="1" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="27.6" customHeight="1">
       <c r="A230" s="1" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="27.6" customHeight="1">
       <c r="A231" s="1" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="27.6" customHeight="1">
       <c r="A232" s="1" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="27.6" customHeight="1">
       <c r="A233" s="1" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="27.6" customHeight="1">
       <c r="A234" s="1" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="27.6" customHeight="1">
       <c r="A235" s="1" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="27.6" customHeight="1">
-      <c r="A236" s="1" t="s">
-        <v>458</v>
+      <c r="A236" s="6" t="s">
+        <v>531</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="27.6" customHeight="1">
-      <c r="A237" s="1" t="s">
-        <v>460</v>
+      <c r="A237" s="6" t="s">
+        <v>533</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="27.6">
       <c r="A238" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>471</v>
+        <v>452</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="27.6">
       <c r="A239" s="1" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>473</v>
+        <v>453</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="1" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="1" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="27.6">
       <c r="A244" s="1" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="27.6">
       <c r="A245" s="1" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="1" t="s">
-        <v>487</v>
+        <v>467</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="1" t="s">
-        <v>490</v>
+        <v>470</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>489</v>
+        <v>469</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>492</v>
+        <v>471</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="1" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="6" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="B250" s="6" t="s">
-        <v>543</v>
+        <v>521</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="27.6">
       <c r="A251" s="6" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="B251" s="6" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="6" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="B252" s="6" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="6" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="6" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="6" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="B255" s="6" t="s">
-        <v>505</v>
+        <v>483</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="6" t="s">
-        <v>506</v>
+        <v>484</v>
       </c>
       <c r="B256" s="6" t="s">
-        <v>507</v>
+        <v>485</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="6" t="s">
-        <v>508</v>
+        <v>486</v>
       </c>
       <c r="B257" s="6" t="s">
-        <v>509</v>
+        <v>487</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="27.6">
       <c r="A258" s="1" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>513</v>
+        <v>491</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="1" t="s">
-        <v>510</v>
+        <v>488</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>511</v>
+        <v>489</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="6" t="s">
-        <v>515</v>
+        <v>493</v>
       </c>
       <c r="B260" s="6" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="27.6">
       <c r="A261" s="6" t="s">
-        <v>516</v>
+        <v>494</v>
       </c>
       <c r="B261" s="6" t="s">
-        <v>517</v>
+        <v>495</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="6" t="s">
-        <v>518</v>
+        <v>496</v>
       </c>
       <c r="B262" s="6" t="s">
-        <v>519</v>
+        <v>497</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="27.6">
       <c r="A263" s="6" t="s">
-        <v>520</v>
+        <v>498</v>
       </c>
       <c r="B263" s="6" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="6" t="s">
-        <v>522</v>
+        <v>500</v>
       </c>
       <c r="B264" s="6" t="s">
-        <v>523</v>
+        <v>501</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" s="6" t="s">
-        <v>524</v>
+        <v>502</v>
       </c>
       <c r="B265" s="6" t="s">
-        <v>525</v>
+        <v>503</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="6" t="s">
-        <v>526</v>
+        <v>504</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>531</v>
+        <v>509</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" s="6" t="s">
-        <v>527</v>
+        <v>505</v>
       </c>
       <c r="B267" s="6" t="s">
-        <v>530</v>
+        <v>508</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="6" t="s">
-        <v>528</v>
+        <v>506</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>529</v>
+        <v>507</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" s="6" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="B269" s="6" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="27.6">
       <c r="A270" s="6" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="27.6">
       <c r="A271" s="6" t="s">
-        <v>536</v>
+        <v>514</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>539</v>
+        <v>517</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="27.6">
       <c r="A272" s="6" t="s">
-        <v>535</v>
+        <v>513</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" s="6" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="B273" s="6" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="27.6">
       <c r="A274" s="6" t="s">
-        <v>537</v>
+        <v>515</v>
       </c>
       <c r="B274" s="6" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>